<commit_message>
Get daily reddit data: Tue Oct  8 08:11:04 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_13.xlsx
+++ b/data/collected_data/2024_10_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C482"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3083 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1fyugw3</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Hello kitty lovers unite!</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9gb6ck7umhtd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1fyu84s</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Did this set for my graduation party</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xd1f44pfjhtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1fysrrm</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>OPI is amazing</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fysrrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1fysnz2</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>BLUE!</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q1glg0duygtd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1fyskna</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>How to grow thin and brittle nails</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ysl4n2anxgtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1fysggx</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>my first set of acrylics!!</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmdox857wgtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1fyr9yy</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>shellac nails</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyr9yy</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1fyn1fo</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>How do you round the tips?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fyn1fo/how_do_you_round_the_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1fyidtf</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Chrome Accents</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyidtf</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1fyemez</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Wedding Nails 💕💕</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyemez</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1fys0s4</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The changing of the guard 👻🎃 </t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fys0s4</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1fyrz91</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>My acrylic nails have broken 4 times in the 2 weeks since I got them</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vx1edq3oqgtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1fyri8l</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you need to take a break on gels? </t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fyri8l/do_you_need_to_take_a_break_on_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1fyrdwu</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>My current set 💅🏽🤍🖤</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwdwrgmyjgtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1fyqgg2</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>I used orlys sec n dry on my natural nails and it peeled off the next day. What did I do wrong?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vgnryyfjagtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1fyqfcw</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cyber-spooky </t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7al29qk8agtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1fypotd</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First full set of gel extensions I’ve ever done </t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bgybr2x53gtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1fypgwn</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall set </t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2mp8dp31gtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1fyoefe</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>snip snip</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyoefe</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1fymg70</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>TW/Gore/ First time trying gore nail effects! (Glass version) How can I make this better? 🤔</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cql83v50aftd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1fynk3v</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bitten nail progress </t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fynk3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1fyn85d</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Halloween/Fall nails🎃</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyn85d</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1fyn7ui</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>I really love the color red on my nails, they are totally natura</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfzs5mlhgftd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1fyn12k</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new super barbie nails! </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87gize91fftd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1fymsrx</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Spooky Season Nails 🕷</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/duw8l0jzcftd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1fymocd</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They're living it up at the H0tel California </t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fymocd</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1fymlre</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>First time doing someone else’s nails besides my own! Let me know how I did (:</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fymlre</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1fymgg2</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New acrylic nail design with semi permanent polish and cat eye effect. Give your opinions. I bring you this design for this season </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7ghyll2aftd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1fym9eg</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Nail newbie but I'm happy with how my attempt at monarch nails turned out 🦋</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ytqol9td8ftd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1fym1e3</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Halloween!!! 🕸️</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69renxji6ftd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1fyfxg7</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails are weak from gel - what to do? </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fyfxg7/nails_are_weak_from_gel_what_to_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1fyhms1</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Broken nail with gel builder. How are natural nails after years of dip and gel? </t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fyhms1/broken_nail_with_gel_builder_how_are_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1fylvgw</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>how to remove glue from press on nails for re-use?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fylvgw/how_to_remove_glue_from_press_on_nails_for_reuse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1fylsd4</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Tried to do my nails for the first time ever — please swipe for left hand result 😩</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fylsd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1fylhim</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Are this okay?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fylhim</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1fyl15o</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetlejuice Beetlejuice Beetle…….  </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4mvqij6yetd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1fykrvf</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Regular polish on dip? Tips please! </t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fykrvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1fykpqf</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>October Nails!</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fykpqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1fyklho</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>New set with a pop nail!</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyklho</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1fyk93g</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my best friend and I got matching nails! </t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cb41t7muretd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1fyk7qo</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Guys always said they liked blue nails and I finally tried them and I agree</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gyddkumjretd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1fyk2pu</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>What product can I use to prevent this? (Natural nails)</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyk2pu</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1fyjvxn</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>I made these a few days ago. Advice? What do they look like?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4eb9rkr1petd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1fyjio3</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>My birthday set💓 if you couldn’t tell, I love pink😇🥰</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ieqd7uv8metd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1fyhfcb</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How would you describe this style of nail art? </t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qy1ywtt6etd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1fyi0dc</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>My hands are beautiful with these nails😍</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mmayp75betd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1fyj8d0</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>my fall set! took four hours!</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwllv8j4ketd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1fyj577</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Halloween nails, loose glitter with gel polish and nail stickers. Any tips for stickers to lay more flat and less lift before top coat?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyj577</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1fyi9a4</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Beginner and would love advice! 💕</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyi9a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1fyhlhx</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Please explain the science behind using magnetic wands for cat eye nail polish</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fyhlhx/please_explain_the_science_behind_using_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1fyhec4</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New chrome powder! Love the color! </t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1019mu7m6etd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1fyh8m1</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Shortie Fall nails in "Got the Blues for Red" by OPI.</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyh8m1</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1fyh5ah</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Time Painting in a Long Time </t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vz4lvawr4etd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1fygz02</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Best STRONG nail polish?</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fygz02/best_strong_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1fygwlg</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of the nail i just made it’s my second time making nails and first time using sod gel extensions </t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fygwlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1fygt61</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>this effect 😍</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eg7h4qgb2etd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1fygp2x</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>I've had my nails done for 20 days, and it's almost time for maintenance!!! I love shades of blue!!</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fygp2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1fygozj</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">18y/o sis in cosmetology school got me right </t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fygozj</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1fygjoy</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is there a way to grow nailbeds? </t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtjjm5oc0etd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1fyghqn</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Halloween nails pt. 1</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/so1rk7jxzdtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1fygamg</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Ghost Vibez</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1iyjm2sgydtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1fyg2vb</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which shape suits me best? </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyg2vb</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1fyfzv8</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 months of nail growth </t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n536pll9wdtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1fyfw4c</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>This was fun…</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzrb4i8jvdtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1fyfmla</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Polygel Brush recommendations for my Wife</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fyfmla/polygel_brush_recommendations_for_my_wife/</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1fyfki0</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Hand painted tortoise shell for fall 🍂🐢</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyfki0</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1fyfajb</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>My new shorties ❤️</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ly8ewsh5rdtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1fyf3lf</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall vibes </t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pi1vzlpppdtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1fyey1x</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>My Beetlejuice nails I did myself</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyey1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1fydts0</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Went for light taupe this time 🦭</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fydts0</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1fydsef</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Nail rings 🤍🩶💚</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fydsef</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1fydmwa</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Purple lines on back of nails?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vrylto43fdtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1fy5u16</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>What do I ask for?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fy5u16/what_do_i_ask_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1fy9bjb</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What happened here?! </t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bowvskaejctd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1fy9cqg</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Creepy crawlies 🐜🦋🐛</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy9cqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1fyd5ya</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Damaged nailbed?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyd5ya</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1fyd3v1</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My DIY Halloween nails 💅 </t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyd3v1</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1fyd2u3</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Manicure today </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyd2u3</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1fycwx8</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love them </t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p63de3dt9dtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1fycwjw</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First try with dip powder </t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bos3m4r9dtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1fyctoo</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Soot sprites 🥰</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyctoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1fyc4g3</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first DIY Halloween nail set! </t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyc4g3</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1fyc0nj</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Did this nails on my friend and I'm so proud</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9gaumv63dtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1fybsfo</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Obsessed is an understatement! Nocturne by Mooncat 😍😍</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fybsfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1fybhzh</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>I cant stop staring at my new nails🤩</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jq1rv5czctd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1fybhfm</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>What do you think about this acrilyc set? Truely ♥️</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrj1yt29zctd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1fyb6ir</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Purple glitter, do you think it's a good choice for october</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyrv00s2xctd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1fyb1pj</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Got my nails ready for Terrifier 3!</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/voyv89i3wctd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1fy9zec</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help!!!! </t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy9zec</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1fy9don</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>ILNP - Bitten</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy9don</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1fy9d9t</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Please don’t kill me Mr. Ghostface</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy9d9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1fy8zg1</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Perfect autumn nails do exist 😍</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m49ihfsugctd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1fy8ipf</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>coquette nails 🎀</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy8ipf</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1fy81nn</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Time for Halloween!! 🖤🕷️🕸️</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy81nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1fy7z3e</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Thin nails look</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fy7z3e/thin_nails_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1fy7v9r</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>My second set…</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy7v9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1fy7m68</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Halloween Set 👻</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpds74636ctd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1fy7e7t</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>home based nail tech client etiquette?</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fy7e7t/home_based_nail_tech_client_etiquette/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1fy7dur</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>My new super shine nails 🤩</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy7dur</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1fy77lx</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>October Nails</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9pee81bp2ctd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1fytxnh</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Chaos skittle (Build a Bear for bg and tax)</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fytxnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1fys9a1</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Horseshoe vs 2 wand magnets??</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fys9a1/horseshoe_vs_2_wand_magnets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1fys5an</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>I literally just finished the mani, am in agony</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddvr31nksgtd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1fys1xv</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Recycling nail polish</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fys1xv/recycling_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1fyrulu</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Fiyero's My Mani</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyrulu</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1fyqsu2</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Put orly sec n dry on my natural nails and it peeled off the next day? Did I mess up?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhxyso90egtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1fyqrue</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Inspired by RC from Toy Story</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyqrue</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1fyprsq</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Color match for PFS Goblins and Ghoulies?</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyprsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1fyp08g</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Note to indie polish makers: if you make a light gray polish with pink shimmer and name it after Moo Deng, I will buy it in a heartbeat</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fyp08g/note_to_indie_polish_makers_if_you_make_a_light/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1fyofjk</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>It Could Happen</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u8bl28hgrftd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1fynpu5</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Bright polish for very fair skin</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqjcnqh8lftd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1fynpr8</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Quick Mani Tips</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fynpr8</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1fynkw0</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Mooncat has done it again. Absolutely wild shift.</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zqxmfrcqjftd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1fyn08g</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>BKL - 9,998,383,750,000 (GWP) over Little Serpent (PPU 8/24)</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyn08g</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1fym6o1</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Red Velvet magnetic franken</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gm5q4cjq7ftd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1fym52t</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>night sky on my nails - magnetic jelly sandwich!</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/au3dkf2d7ftd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1fylmgs</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>BKL - 9,998,383,750,000🍂</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fylmgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1fyl8t2</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Tried out I swell with some flakes on top</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyl8t2</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1fyk8c7</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Ethereal Vampire slaps 🥀</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/631ji9roretd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1fyk40r</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Halloween week 2</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvxvg8qqqetd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1fyjffn</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Traveling to Japan, please help!</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fyjffn/traveling_to_japan_please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1fyjcx7</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>My first time doing nail art!!!</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyjcx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1fyj96r</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>First two weeks of October feel like such a Waste of Space! ☄️👻</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyj96r</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1fyj6qb</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Any dupe of Mooncat's Twilight Sonata?</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dkfqdwsjetd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1fyiv0y</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>My new favorite polish!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyiv0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1fyitul</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>These Polishes Are Out of Thos World</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyitul</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1fyirpn</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Shifty beauty from Prism Polish!</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyirpn</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1fyiamo</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Mooncat- Garden of Evil</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyiamo</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1fygq6v</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>help with stamping appreciated</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10yh537p1etd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1fyfcon</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Any ladies have pics of wearing Rouge Rockefeller - Cirque Colors?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fyfcon/any_ladies_have_pics_of_wearing_rouge_rockefeller/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1fyfasf</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>I don’t think a wrap will save this one 🥲</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kaalnhe7rdtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1fyf186</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Spooky season marble &amp; gradients</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h69g5396pdtd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1fyer90</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you find that Seche Vite actually performs better than other quick dry top coats? Or are most of them pretty similar with how quickly they dry?  </t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fyer90/do_you_find_that_seche_vite_actually_performs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1fye5ky</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Return to Polish - Quick Routines? </t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fye5ky/return_to_polish_quick_routines/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1fye0l2</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Nails for a hands-on job and to help curb skin picking?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fye0l2/nails_for_a_handson_job_and_to_help_curb_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1fyds86</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Cottagecore sticker dream!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cf8k9s66gdtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1fydckx</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grave ghosts at the consequences gate </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fydckx</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1fyd8ma</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PSA before heading to Ulta for Holo Taco: "available in stores" but not for pickup = you're in luck! ...but not yet (call ahead before trekking out). + swipe for presumed initial locations in Mass &amp; NH </t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyd8ma</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1fyco6m</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My French Mani I did last week </t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyco6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1fycabf</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Comparing some of my light pink holos </t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fycabf</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1fyc17w</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How Do I Unread This? </t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eealpyqa3dtd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1fyby1e</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Best pinks for sparkle lovers?</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fyby1e/best_pinks_for_sparkle_lovers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1fybsve</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is Stolen Ambrosia the perfect Autumn shade?? I think YES </t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lc5q5rkl1dtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1fybhy8</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Spooky season</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fybhy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1fyb77c</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Crystal Knockout 25 fly</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyb77c</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1fyad7u</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Ethereal Nocturne- a fall nude with some attitude!</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/guntdpgwqctd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1fya8e9</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>First Mani With A Cleanup Brush!</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22edj906qctd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1fya84n</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>DVN Halloween 2024</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fya84n/dvn_halloween_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1fy9jfx</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>BKL- The Woman In Black</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy9jfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1fy9hhb</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Cirque “Luck Jelly” might actually be lucky 😋</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy9hhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1fy9f2p</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>ILNP - Bitten</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy9f2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1fy87yb</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>How long would it take you to use your whole collection?</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fy87yb/how_long_would_it_take_you_to_use_your_whole/</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1fy7tup</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Anyone else having trouble with olive and June delivering their nail polish?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fy7tup/anyone_else_having_trouble_with_olive_and_june/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1fy7bll</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>HT/MC Releases</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fy7bll/htmc_releases/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1fy6k5d</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>big flakies addicted</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy6k5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1fy62m9</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t xml:space="preserve">From ✨shiny ✨ to matte </t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy62m9</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1fy416d</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fy416d/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1fy30av</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I stop nail art looking bulky and bumpy on my nails? </t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fy30av/how_do_i_stop_nail_art_looking_bulky_and_bumpy_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1fyuknz</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Flowers and feathers</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyuknz</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1fysnfn</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is how I humbly practice my nails for 🎃 </t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptgh0upnygtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1fyq3vu</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Black &amp; Chrome Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyq3vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1fypfc0</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall set </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsegmruo0gtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1fyowq4</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Halloween So Far</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyowq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1fyojqv</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Trying Walmart Chrome!</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2e5x7a9msftd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1fymfux</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>TW/Gore/ First time trying gore nail effects! (Glass version) How can I make this better? 🤔</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70tq6e6x9ftd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1fyiwcf</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Clear top coat smudging black nail art </t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fyiwcf/clear_top_coat_smudging_black_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1fyih9v</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Booh Nails👻</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtyz4r3leetd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1fyievt</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Soft Color</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06cd2lc3eetd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1fygwrp</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Pink Frenchies</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59t3ot123etd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1fygrp3</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Yay spooky season!</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ww6yhz5y1etd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1fygqsc</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>💀👻🎃</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fygqsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1fygmp4</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Beetlejuice nails I did myself </t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fygmp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1fyfr03</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Artsy tingxzzz YOUR GIRL IS PROUDDD</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyfr03</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1fyf54x</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Nails b-day</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrne4rl1qdtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1fyd6fw</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of my work? Would you pay for it? I'm afraid to take the plunge </t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyd6fw</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1fyb04s</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Ready for Terrifier 3!</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy2x4azrvctd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1fy8x68</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Please don’t kill me Mr. Ghost face</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy8x68</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1fy847m</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Fall nails 🤎🧸</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy847m</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1fy7ody</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>halloween nails :)</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy7ody</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1fy3b3u</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Please recommend me a strong magnet for cat eye!</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@rayabeautynail/video/7162044970768059654?lang=en</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1fy2wco</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Has anyone ever experienced the Day of the Dead festival? Give me a thumbs up if you'd like to try visiting Mexico for it!</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fy2wco</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Oct  9 08:10:30 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_13.xlsx
+++ b/data/collected_data/2024_10_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C482"/>
+  <dimension ref="A1:C639"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8627,6 +8627,2675 @@
         </is>
       </c>
     </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1fzm9vx</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Been loving my new colour combination!</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzm9vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1fzm3f0</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Art cute enough to keep?</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzm3f0</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1fzlhtf</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>First attempt at chrome... kinda messy but still pretty!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nsoc4auaiotd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1fzlcef</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My friends work! </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54i6s2u8gotd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1fzjz6x</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Do I have press-on nail blindness?? This is my second try at them and I actually like how they turned out!</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzke0vjoyntd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1fzjnmh</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Cats eye</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fzjnmh/cats_eye/</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1fzjhil</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Can I put the nail back on?</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nr0isu30tntd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1fzjcku</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>My autumn nails 🥹</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2r40wu4grntd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1fzixy8</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>OMG!! I love this soooo much 🧚🏻‍♂️💖</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzixy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1fzi5mt</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>my third set of nails ever! kinda proud</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwv6938qentd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1fzi8ar</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love doing touch-ups, it's been a month since the design was done and it's as good as new, what do you think? </t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzi8ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1fzi5bm</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky little ghosties with a wall of souls accent </t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzi5bm</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1fzi3w6</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | HHC - Shiftcraft</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzi3w6</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1fzhonb</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Painting American Horror Story nails for halloween- Here is Tate! Violet coming soon 💕</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/um2l5qz2antd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1fzhoam</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Painting American Horror Story nails for halloween- Here is Tate! Violet coming soon 💕</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b7wy8idz9ntd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1fzhec1</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>New pressons from toaboa 😍</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2utm9vcb7ntd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1fzhdmu</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Simple fall-ish florals</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/KDWn07E.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1fzhbtb</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Day and Night</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzhbtb</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1fzhbgb</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How should I do my nails tomorrow? </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hn2jwcui6ntd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1fzgw8h</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Do you like them?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kj53d9vg2ntd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1fzgpe1</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Sweater nails with stickers?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ez3kx3op0ntd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1fzfoen</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Coraline and Other Mother </t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzfoen</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1fzf0p4</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my own coralline Halloween nails! </t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzf0p4</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1fzeywz</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzeywz</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1fzew05</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rate my nails </t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uehpl0sxjmtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1fzep4w</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t xml:space="preserve">question: new to diy nails </t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fzep4w/question_new_to_diy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1fzenug</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>"Lookit, lookit! It's fricken bats. I love Halloween"</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzenug</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1fzekb3</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Fresh nails 💜</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjct7n43hmtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1fzeal0</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Thinking about doing a doll makeup on my hand</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ft38wzvqemtd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1fzcu36</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Builder gel FTW</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzcu36</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1fzdb37</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Shaping press ons - possible??</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f33nyyj76mtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1fzd68z</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t xml:space="preserve">halloween nails 👻 </t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzd68z</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1fzcru7</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivcyhpks1mtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1fzcolt</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>My spooky nails, all painted by hand!</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzcolt</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1fzckhn</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My cutie little cat eye starry skies for Halloween </t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8tx8tf20mtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1fzatrl</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pop art nails </t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzatrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1fzakul</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Builder gel and Rubber base chipping and peeling off?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ufvf7idkltd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1fza5cg</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Spooky season is upon us</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fza5cg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1fz9usq</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t xml:space="preserve">short nails~ pochacco and cinnamoroll </t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz9usq</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1fz9ns9</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Natural nails, trying out new products !</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz9ns9</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1fz9m92</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Clown nails 🤡 </t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz9m92</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1fyuc0u</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>What is this on my 4 day old acrylics?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyuc0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1fymjod</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Inspo</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gcv5u5ouaftd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1fz6oub</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>my spooky hand painted press-ons 💅🏼🎃</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz6oub</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1fz91vo</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Suspicious about my inspo lol </t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/um6ujoft8ltd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1fz94da</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Clear tips with encapsulated red flowers</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz94da</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1fz8w39</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>What do we think about these press ons?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yo39rnil7ltd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1fz8v5o</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t xml:space="preserve">one of wun - Gunna </t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz8v5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1fz882d</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Press on nails :)</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz882d</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1fz811t</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural Nail Rehab Help </t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz811t</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1fz7xfr</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>I fell in love, although they look exaggerated, would you make them?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpyxma490ltd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1fz7jbx</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just got my gel nail polish removed &amp; my nails feel so fragile </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/csstnddfxktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1fz7iqr</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Autumn Pumpkins 🍂🎃</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz7iqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1fz6vpl</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Thumb is 1mm too big for custom press on, is that a big deal?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fz6vpl/thumb_is_1mm_too_big_for_custom_press_on_is_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1fz62fk</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you think they’re boring? </t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgaimv5gmktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1fz5x95</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Holo Taco Display Rack (Storage Solution?)</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fz5x95/holo_taco_display_rack_storage_solution/</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1fz5g5k</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>First time using builder gel and woooow 🤩</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5nat7fuwhktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1fz506s</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>First time doing gel X and cat eye nail polish 💅✨️</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz506s</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1fz4pk3</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>This was my favorite nail design 😍</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69ht59hgcktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1fz1l4s</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Engagement nails inspo?</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fz1l4s/engagement_nails_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1fz1lso</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Neutral gel set I did on myself 🕷️☁️🎱</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8tpbyafpjtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1fz3hql</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Feminine hands at last!</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/buakh3he3ktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1fz3fpv</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Shein will do, these press ons lasted through and beyond a 1.5 hour dumbell session</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8tdqte03ktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1fz35l6</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>spooky season!</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz35l6</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1fysji0</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Need suggestions for dusky skin</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fysji0</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1fz2cte</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Tips for filing natural nails (pics included)</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fz2cte/tips_for_filing_natural_nails_pics_included/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1fz1ybe</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Did these yesterday 💖</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz1ybe</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1fz1fr9</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aruba Blue </t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz1fr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1fz16ue</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Best Full Cover Nails and Glue</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fz16ue/best_full_cover_nails_and_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1fz14u6</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>This time i tried to do my own nails🌹✨</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz14u6</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1fz1372</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>How to get my gel nails to stop peeling off?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fz1372/how_to_get_my_gel_nails_to_stop_peeling_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1fz07e4</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>That shineee</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q16elkqfejtd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1fyzu2t</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>What suits me better?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyzu2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1fyz3el</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>First time doing nails in months!</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyz3el</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1fyyycb</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t xml:space="preserve">12 years ago my mother taught me to do nails. And today I finally had the honour of doing hers! </t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eder2ooq3jtd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1fyyl69</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>October Sally nails 🎃🧡</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwkabi0h0jtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1fyyfj7</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t xml:space="preserve">do these look like press-ons? </t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyyfj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1fyy3dw</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thought I’d share some of my nails from when I was a bartender </t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyy3dw</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1fyxy1e</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Mt favorite nail polish in the winter 💅</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uutgpjabuitd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1fyxojf</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>OBSESSEDDD</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyxojf</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1fyvc6x</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Obsessed with cat eyes!! Also, do you think an almond shape would suit me better?</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3ddwb5m6zhtd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1fzkq9s</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>That girl is Poisooooon</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3adm5z908otd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1fzk6gt</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some velvet nails </t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/imuweo131otd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1fzjy7k</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hypnotic Polish Experiences </t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fzjy7k/hypnotic_polish_experiences/</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1fzjk7y</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another matching set </t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8g9o1ivtntd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1fzipqw</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>If you’ve ever wondered what happens if you get a nail stuck in your keyboard…</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkf42nwjkntd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1fzilmo</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Nightcrawler 🔮</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzilmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1fzi2il</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | HHC - Shiftcraft</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzi2il</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1fzhm7x</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>NFU OH 51</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzhm7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1fzhdkb</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sagebrush by mooncat 🌙 🌟 </t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzhdkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1fzgd3k</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Poison</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzgd3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1fzfiue</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polished For Days - Grave Consequences </t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzfiue</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1fzfiix</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Hard as Hoof Cream and Polish Lifting?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fzfiix/hard_as_hoof_cream_and_polish_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1fzfc11</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Essie’s Berry Naughty for October 🍷</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzfc11</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1fzfbwq</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>We all have polishes that we love, but is there a collection that you're obsessed with?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fzfbwq/we_all_have_polishes_that_we_love_but_is_there_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1fzf9kr</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Dead Girl Nails for Spooky Season</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aeozyjeenmtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1fzeya8</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Cirque Delusions of Grandeur ~ Lazy Cat eye</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oawlvugekmtd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1fzev8e</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Was in the mood for something neutral/subtle. Thoughts? </t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzev8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1fzekrr</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Vintage Avon Dupes</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fzekrr/vintage_avon_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1fze40b</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reaching skyward </t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fze40b</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1fzcp3h</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>The Magic of Hidden Potential</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzcp3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1fzck6m</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>september mani dump 🍂☕️</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzck6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1fzbrtn</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>BKL freebie - I Believe it was Dostoevsky that said, Later F*cker</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzbrtn</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1fzb0mc</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Similar to OPI Gel Let's Be Friends! By Hello Kitty ?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fzb0mc/similar_to_opi_gel_lets_be_friends_by_hello_kitty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1fzaj25</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Chanel Peridot dupe in a gel?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fzaj25/chanel_peridot_dupe_in_a_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1fzabcy</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tips to prevent peeling nails? </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fzabcy/tips_to_prevent_peeling_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1fz9clp</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Cirque Delusions of Grandeur (velvet)</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t0204w80bltd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1fz86o2</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My take on fall nails </t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz86o2</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1fz81sm</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural Nail Rehab Help </t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz81sm</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1fz712w</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>First ILNP Experience</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz712w</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1fz6zan</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Ghosts at the Gate</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pke6369atktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1fz6uy0</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Spooky Halloween 👻 "Glamermaid"</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz6uy0</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1fz6la9</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Cirque must haves for fall/winter?</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fz6la9/cirque_must_haves_for_fallwinter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1fz6gfs</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Fall haul!</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpvrtnzapktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1fz5zkp</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Mooncat bottles with seams in my order</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz5zkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1fz5xz7</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Little Skittle Action!</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52qifvqjlktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1fz5pih</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Glass nail files…</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fz5pih/glass_nail_files/</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1fz5514</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>First time using builder gel and woooow 🤩</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rhi69tfmfktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1fz529n</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>My Durga Puja Special Nail Lacquers</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz529n</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1fz4x45</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>DVN Golden Smog</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ys7rsfezdktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1fz4qxu</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Posted earlier but the color looks so much brighter under fluorescent lights! My best job yet in my DIY nail journey </t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz4qxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1fz4qls</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone else’s Vibrant Scents top coat turn yellow? What could be the reason for this? </t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz4qls</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1fz4hfw</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tips on capping the free edge? </t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fz4hfw/tips_on_capping_the_free_edge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1fz45hn</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>How to duplicate this look?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fz45hn/how_to_duplicate_this_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1fz3udw</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Tyler's Trinkets I'm Smad + topper and Re-Animated</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz3udw</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1fz38c0</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>OPIxWicked Fiyero’s My Mani &amp; I’m the Wonderfullest</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz38c0</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1fz325a</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Boogeyman- Ahmaya cosmetics </t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz325a</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1fz2ftg</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Dammit Janet (I love you)</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcanqvmmvjtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1fz2dwn</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Name that Prune- not prugly at all!</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz2dwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1fz19h1</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Impressed with Cracked Polish</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz19h1</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1fz11z0</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>“Mint Chip Madness” by Painted Polish</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5537fx5ljtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1fz0zch</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Is there any way to fix this?</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz0zch</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1fz0tir</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Birthday mani</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u59tqh0cjjtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1fyze7f</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not a fall color but I love a good pink </t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyze7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1fyy50q</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetles e572 </t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyy50q</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1fyy00e</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>I'm not normally a flakie girly, but this polish is changing my mind!</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyy00e</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1fyxptu</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Loving this 🧡 (OPI, ILNP, Phoenix Polish)</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fyxptu</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1fzkopr</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Don’t jump it’s just a nail spider 🕷️ </t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t4vap1nh7otd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1fzhp1n</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Painting American Horror Story nails for halloween- Here is Tate! Violet coming soon 💕</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/268qyky6antd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1fzhowf</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>This week set ✨</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzhowf</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1fzh7g5</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails inspired by pics on Pinterest </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8efax8h5ntd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1fzgknz</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Trying Walmart Crome pt. 2!🍏🍏🍏</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k2rdzlwfzmtd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1fzfxva</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ghostface inspired halloween nails </t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hd0l4iitmtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1fz99c1</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>i love halloween the nails are always so fun!!!! and i absolutely loved making georgies little boat!</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz99c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1fz92a2</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Clear tips with encapsulated red flowers</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz92a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1fz8rcg</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Two weeks later survived daily life</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz8rcg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1fz87w2</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my nails for some Twenty One Pilots concerts, lmk what you think. </t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz87w2</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1fz7720</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Amateur Hour</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz7720</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1fz6vl0</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>A wedding set</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz6vl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1fz6juz</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>New set of press ons from b.e.nails! Halloweenie 🎃</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x25gn2ftoktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1fz6euc</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Faded leopard print nails?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7wnegczoktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1fz4sx9</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>didn’t get much love on another sub so i’m sharing here!</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v72fixx3dktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1fz4177</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Junk nails are my weakness </t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovsdplrf7ktd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1fz1i4u</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>1st Halloween set!</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fz1i4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1fyyhjq</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Spooky szn part 1</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/37w9f78izitd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1fywzbx</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Thoughts of nail art for men? Check out these flames 💅🏻🔥</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgwsyef7kitd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1fyv7g2</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>first time doing nail art</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41u3xopcxhtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Oct 10 08:10:38 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_13.xlsx
+++ b/data/collected_data/2024_10_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C639"/>
+  <dimension ref="A1:C825"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11296,6 +11296,3169 @@
         </is>
       </c>
     </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1g0dt8i</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>my spooky nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0dt8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1g0drkr</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sometimes we need to come back for the classics... With a twist </t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0drkr</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1g0dnzs</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Witchy ombré for Halloween.</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0dnzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1g0dhg1</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>I’ll never forget walking into  the nail salon as a first time customer and asking them if they could hand paint Art the Clown on my nails. They said, we can do something similar. How’d she do?!</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gn7qbsaduvtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1g0cyw2</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recs for a Seattle private nail tech? </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g0cyw2/recs_for_a_seattle_private_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1g0cr3w</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>painted my nails for the first time :)</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2obeicbkvtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1g0c0xz</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pumpkin nails for autumn 🍂 </t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0c0xz</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1g0bod9</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>My very, very amateur spooky nails ❤️</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0bod9</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1g0bleg</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>What type of nail shape would suit me best (f)</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nkju71b5vtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1g0bhkl</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Spooky season is here!👻</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glzmlsh04vtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1g0bdfc</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Brown yay or nay?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0bdfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1g080kq</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel-X set 🕷️ </t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvgyie0m3utd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1g0az4a</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>My first spooky set!</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0az4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1g0as0q</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Acrylics turned upwards</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0as0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1g0amh7</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Been doing my own nails for 1 year, is there any advice for smooth gel application?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0amh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1g0aamd</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Nail lamp multipurpose..?</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g0aamd/nail_lamp_multipurpose/</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1g0a5g8</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>What type of nails is best for me?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0a5g8</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1g09vo1</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Natural Nails</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g09vo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1g09qz6</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>are my nail beds too small or it's just the nail being long</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g09qz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1g08mgv</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mystical Vibes </t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g08mgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1g08i60</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Is it possible to get a nail tech license as a teenager?</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g08i60/is_it_possible_to_get_a_nail_tech_license_as_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1g08fj8</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Wanted to share my spooky nails too ✨done by me✨</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0s6vz2i7utd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1g07str</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Halloween fever</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g07str</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1g06sjb</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Clouds</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0h3hgvq8sttd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1g06qm0</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Beetlejuice Beetlejuice BEETLEJUICE!!</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g06qm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1g06mb1</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Candy apple red for Halloween 🍎</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g06mb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1g06fl5</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Feeling Fall Vibes🍂🍁🍂</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fr2y62rzottd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1g06ar9</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Can I fix this or am I gonna have to trim them all? 🥲</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuh0bcfsnttd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1g05nxx</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky birthday nails </t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g05nxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1g05lxi</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These insanely pretty press ons!! </t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g05lxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1g051sb</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Ghost Nails</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8elf8h7vcttd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1g043ci</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My dream mermaid nails!🧜🏽‍♀️ </t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g043ci</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1g03xwe</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>I made some stainless steel nails!</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g03xwe</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1g03s2d</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How often does everyone get their nails filled? </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/td6evasb2ttd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1g02h3o</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I hate my nails and idk what to do now </t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g02h3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1g031z1</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Trick r Treat inspired nails!! I’m so in love!</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g031z1</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1g036yt</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Spooky nails</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8e84jznnxstd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1g035ib</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dry Nail Polish rubs lines on surfaces </t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g035ib/dry_nail_polish_rubs_lines_on_surfaces/</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1g02wpc</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Try Week-Old Tortoiseshell (Cheetah print?) Nails </t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvefqlwevstd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1g02q7h</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>halloweeny vibes!!! 🖤</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g02q7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1g02mlo</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>First fall nails</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g02mlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1g02i7p</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>What's best for AcryGel?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g02i7p/whats_best_for_acrygel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1g00ox5</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Question RE: Time between manicures</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1fpzq1eestd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1g010h9</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>I’d love to learn!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g010h9</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1g01287</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails in jeans! </t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g01287</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1g01d4z</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>2.0 Linkin Park "From Zero" Album Art Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2s8gkmlfjstd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1g01qvr</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>I have finally achieved the glazed nails with nail lacquers</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/teu1xklfmstd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1g01p7w</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Glossy pink nails. Loving this soft and classy look:)</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ol57ggtklstd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1g01ea8</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>For those in denial about the end of summer...</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g01ea8</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1g019gh</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Doh!!!</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvhrlbkristd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1g00mfg</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Getting into the fall spirit and did orange w/gold glitter top coat 🍂</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g00mfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1g00i3o</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>All the bio gel nails I’ve gotten done this year so far</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g00i3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1g00ft7</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Hand painted!</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g00ft7</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1g00col</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails </t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g00col</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1g00558</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This year’s Halloween Nails!🩸 </t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kiergu7bastd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1g006xb</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting mine done how did she do?! </t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mcrzsuoastd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1fzyb2o</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>My October manicure is set    👻🎃🦇🕸️! My nail tech did great! ➡️Inspo pic</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzyb2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1fzyuik</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Does anyone know where I can purchase more of these beetles nail tips?</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvz6cffi0std1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1fzziry</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails 💅 </t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzziry</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1fzzhrf</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>I feel so feminine with this design</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjze0p4f5std1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1fzzarg</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Fall nails🍂</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwlmv82z3std1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1fzz787</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Birthday nails 🌌</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzz787</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1fzz68h</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t xml:space="preserve">art prompt was “apricot” - what do you think of my attempt? :) </t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49k7yse23std1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1fzz4es</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Always love Halloween nails! 👻</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2m91n8o2std1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1fzyjpb</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>My attempt at some spooky nails</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qn1xb49yrtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1fzxvd4</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Jump scare</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyhj9y46trtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1fzxo1m</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Kiss XL press-ons with a little added razzle dazzle…</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ci8z877qrrtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1fzx4yl</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>I am a beginner, what's my worth?</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzx4yl</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1fzx1mb</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22kyvhp1nrtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1fzwyir</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>thinking about starting by selling nails to friends, how can I know how to price my work?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzwyir</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1fzwfn4</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>toughest nails technique?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fzwfn4/toughest_nails_technique/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1fzwdb0</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t xml:space="preserve">attempted some Halloween nails, nail art is stressful </t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6l7za71irtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1fzw4el</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Nails done by myself, what do u think? :)</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yubuy9y4grtd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1fzvznl</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>🤔 I guess it doesn’t look too bad</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j50z5b4afrtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1fzvtcr</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple Chrome and Matte Black </t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jutpwv4zdrtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1fzvr7d</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Would you add anything? </t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91un7o7jdrtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1fzvpd3</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Got a nice shape and length now, What should I do with them?</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jsub3n45drtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1fzvhqx</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Picked out two colors</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3d1lqh8kbrtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1fzvghh</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>What shape should I shape it into?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzvghh</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1fzklsp</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>My Idea VS What I Got! (Nails done by nailsbysophia99 on IG)</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzklsp</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1fzsw6s</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>I’m fall-ing for these Nails!</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzsw6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1fzmunt</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Second set of press ons!</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzmunt</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1fzsaqe</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Fall mani</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzsaqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1fzuj8v</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My gel-x manicure I did last night it’s pink so I love it ft: my mostly eaten pb&amp;j </t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7dxvtnf4rtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1fztyul</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>What do we think? Gel-x</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fztyul</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1fztxzc</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What am I supposed to do with this?? </t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fztxzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1fztvll</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Halloween graveyard nails</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://imgur.com/gallery/rhCoof2</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1fztue6</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>What color?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yyu9fx8zqtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1fztmmb</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Bordeaux</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wy8e14rlxqtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1fztd5y</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do I feel like something is missing or extra? </t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbnfqllovqtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1fztbpy</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>First time trying nails on myself</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9iso8cdvqtd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1fzt4ud</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Tried making my own decals! Success, I think!</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzt4ud</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1fzszct</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Fresh autumn set</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46rk9nhosqtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1fzqzdc</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>What is your go to color?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fzqzdc/what_is_your_go_to_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1fzqlkp</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Left hand or right hand? </t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzqlkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1fzqkry</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>My first attempt at tortoise shell!</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3r2trhq8qtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1fzqe1l</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>5 senses</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzqe1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1fzpztr</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Question about builder gel</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fzpztr/question_about_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1fzpyp7</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>I’m a beginner and have only been doing this about 4 months but I  just cant seem to find an acrylic powder or biab that matches my skin tone! They’re all too light, too pink, or too peachy and it just doesn’t look right… can you recommend any to try?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bk452weu2qtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1fznmrh</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>My spooktober nails</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9zocyjgcptd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1g0cb49</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Can someone explain what the heck happened?!</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0cb49</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1g0bc0x</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Does this look okay to use? (The Willis, PPU Sept 2024)</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0bc0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1g0av6i</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Help with shaping nails/annoying little side bits?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0av6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1g0a4n5</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>first time painting my nails with a non-pink polish !</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0a4n5</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1g09wct</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>This is gorgeous but I don’t want to wait 2 months. Dupe somewhere?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sesz5us2mutd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1g09tru</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t xml:space="preserve">She’s a soft spooky </t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g09tru</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1g09hr7</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooders </t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g09hr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1g08m8z</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Sleepy Vibes Only 😴</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15fcf8ra9utd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1g086ks</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maybe my favorite set I’ve done ✅ </t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g086ks</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1g07r5w</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>do you budget for polish?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g07r5w/do_you_budget_for_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1g072i9</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Such a shocking pink, makes me feel so pretty!!</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jjz6cqsuttd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1g0710x</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>True-to-color glossy topcoat reccs?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8yavwrfuttd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1g06q3g</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Cirque Delulu Collection 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cq22k20nrttd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1g05pzj</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Glittery goblin ✨️</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zoh3whlpittd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1g04yfp</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>10 month grow 🧛‍♀️🩸</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g04yfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1g04lc1</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>“Ghosts and Angels”</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mq2pz5e29ttd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1g04k2d</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Do we need another velvet hack?</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/another-velvet-option-8NWDgf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1g04cy8</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I say something before paying about the cuts? </t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p066c9947ttd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1g03wv7</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Fall mani😊🍷🎃</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g03wv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1g03cyy</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Over the top for wine tasting </t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g03cyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1g030bf</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>My Clionadh Cosmetics anniversary order arrived today and I’m so happy - I gotta share it with you!</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g030bf</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1g026tw</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Mooncat subtle halloween mani</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g026tw</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1g01xky</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Mooncat order, have you tried these shades?</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g01xky/mooncat_order_have_you_tried_these_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1g01x2n</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Cannot stop getting distracted by this shift ✨</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9b8a2q2qnstd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1g01qzb</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Autumnal skittle</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmwcwfbgmstd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1g01h8j</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Folie á Deux</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g01h8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1g019i7</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Matte top coat cracking - why?</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjit0jqristd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1g011bm</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Help finding a dupe for Orly Color Amp’d in Art Walks. Thanks!!</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dp45vvs0hstd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1g00ftv</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Some serious autumnal shiftiness</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g00ftv</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1g00c3s</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Im not sure I really like this color</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g00c3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1g00b9n</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's like spooky season threw up on my nails...... But in a good way.... I think. </t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g00b9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1g007tj</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some cryptids in a foggy forest. Attempt one. Any tips on taking pictures of dark nails? These look so much nicer in person. </t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g007tj</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1g006p1</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Loch Ness</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ovzh5rxmastd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1g000as</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Red French Tips! ❤️</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g000as</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1fzzl15</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>ILNP Venom in 2 coats :&gt;</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/832i9bgy5std1</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1fzynab</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>First Magnetic Mani !! - Sassy Sauce Wicked Sorcery</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fzirjko0zrtd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1fzyjoq</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Spooky Halloween mani, might be my fav I’ve ever done!</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/an1sz809yrtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1fzyckz</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers Contentment</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhgf0f3qwrtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1fzy8ek</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>So Prugly It’s Fugly</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzy8ek</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1fzy7b6</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Goth nails for October</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzy7b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1fzy65a</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Highline is perfect for a fall hike </t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzy65a</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1fzxu2l</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>💛🤍Candy Corn🤍🧡</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzxu2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1fzxjoc</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Finally Fall! 🍁</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzxjoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1fzxh8n</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Indecisive fall mani</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzxh8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1fzx475</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall nails! </t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzx475</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1fzx1d4</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Phoenix Mistress</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/55jecp3ymrtd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1fzwnqt</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I can’t stop looking at my nails </t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzwnqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1fzwkxs</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Can never say no to a one coat vampy</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/we57isykjrtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1fzwjks</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Nailed It! Nail Polish Scarlet Ember</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzwjks</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1fzw7wc</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>This glowy even before topcoat 🥲</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6hitvpygrtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1fzw1xk</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>How do we feel about this Halloween nail art?</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzw1xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1fzvwer</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Fancy Gloss Question</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fzvwer/fancy_gloss_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1fzvgjs</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Cirque Enchanted, I love it!</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzvgjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1fzv4jp</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>This is Some Boo Sheet 👻</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzv4jp</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1fzv0qp</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quick dry top coats keep giving me shrinkage at the tips? </t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fowjd7428rtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1fzuy3i</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>post-gel nail advice</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fzuy3i/postgel_nail_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1fzuwnt</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Love this one more than I thought I would - ILNP First Dance</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzuwnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1fzun1y</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First ILNP order! </t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7b1vg6e85rtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1fzu9m5</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>electric blue flower power ⚡️🌸💅</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzu9m5</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1fztxka</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Antique Spooky Vibes from Velvetine</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fztxka</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1fztqk0</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>🕷️Spooky Nails🕷️</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fztqk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1fzryvq</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Headless Horseman</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzryvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1fzrys6</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>pink and green holo moment</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzrys6</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1fzry31</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>ILNP Haul</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzry31</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1fzrqea</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Trying my hand at gelpolish</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzrqea</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1fzqq4n</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Help me recreate this. I need recs for a light nudie brown for the base, and the medium nudie brown. Thank you.</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>http://i.imgur.com/r2QpL.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1fzqnq7</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>First time trying Maelstrom and wow!</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1r8iikih9qtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1fzqmul</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Shifty show off and a cursed pose for spooky season</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzqmul</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1fznkuh</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Starting my polish journey</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fznkuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1fzmhud</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a Similar Shade —Any Suggestions? </t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzmhud</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1g09o19</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>My try at some ghost nails 👻🖤</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g09o19</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1g05lmn</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Current nails 💅 </t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g05lmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1g04msx</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Fall nails!</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g04msx</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1g01kgg</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>A set I did for myself today!</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g01kgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1g00776</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This year’s Halloween nails! 🩸 </t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qptfk7yqastd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1fzyzm9</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Just take your time</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hj7fijnm1std1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1fzyofp</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute Halloween gel nails </t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzyofp</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1fzwp6d</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Thoughts on my take on ghostface nails?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zq836ofkrtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1fzuxpy</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>What do you think of this nail set?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s3j6gwcd7rtd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1fztwx3</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Halloween graveyard nails</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://imgur.com/gallery/rhCoof2</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1fztw86</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky Halloween 👻 
+</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fztw86</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1fztsbg</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Hocus Pocus nails!</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zx14mfwsyqtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1fzt5yg</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY nail art decals! Success! </t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzt5yg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1fzoxjq</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>coraline nails ✨️🎇 practicing my nail art and 3d skills.</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzoxjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1fzoqlu</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Totoro Nails</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzoqlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1fzn4p0</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween themed press on nails 💅 🤪 ✨️ 😍 💕 ☺️ 💅 </t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fzn4p0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Oct 11 08:10:44 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_13.xlsx
+++ b/data/collected_data/2024_10_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C825"/>
+  <dimension ref="A1:C1003"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14459,6 +14459,3032 @@
         </is>
       </c>
     </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1g148z4</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Second time doing press ons</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g148z4</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1g13imm</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Give me your opinion on my work </t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g13imm</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1g13gao</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>I am a rookie learning to do my own nails- these feel so fresh to me. Yay or nay y’all?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rg2w84dm2ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1g13dur</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginner gel polish and foils - hit me with your comments! </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g13dur</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1g12wzm</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Obsessed with my new Halloween pressons!!</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g12wzm</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1g11yoh</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Supportive husband post.</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g11yoh/supportive_husband_post/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1g114t0</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Bio seaweed gel?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g114t0/bio_seaweed_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1g11967</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Loved these online...on me idk</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g11967</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1g1158r</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second guessing the sparkle ✨ </t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/01b05bt3v1ud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1g111w4</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>How to practice Gel X application?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g111w4/how_to_practice_gel_x_application/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1g10vrx</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my nail tech </t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bq2zbl4as1ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1g10tjx</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Natural nails + biogel!</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ce845jxmr1ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1g109n6</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>This is my favorite red polish ev</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g109n6</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1g106k2</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Tortuous shell vibe, but gold and black</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g106k2</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1g0zqc7</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cow nails maybe French </t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0zqc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1g0zkux</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A set I did for me and my sister </t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0zkux</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1g0zj6b</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my mom's nails today! She loved them! </t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yaf6z43re1ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1g0zef1</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>The most beautiful nails in the world ❤️</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0zef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1g0ze8j</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>I'm obsessed with my Halloween nails!</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0ze8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1g0z6j5</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My last few sets </t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0z6j5</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1g0tho1</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Extremely damaged nails</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g0tho1/extremely_damaged_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1g0xjap</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Fun fruits Nails</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0xjap</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1g0z3yn</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Honest opinion, advice for improvement is welcome🙌 </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4flzm1dsa1ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1g0yymo</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall Nails!!!! </t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03u0nrzb91ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1g0ys93</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>I thought he would be flattered, 😢</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0ys93</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1g0ybko</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Halloween cookie nails!</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w56uk12231ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1g0xqij</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Best press on nails?</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g0xqij/best_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1g0wi16</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>diy draculaura inspired halloween nails 💖🖤🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8b4x9p4m0ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1g0wsy8</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>This years ✨spooky set✨</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0wsy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1g0waj9</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Best affordable gel polish recommendations??</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g0waj9/best_affordable_gel_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1g0vzz1</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Why are powder acrylic nails so thick?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0vzz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1g0scwy</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>My new Halloween nails!! I am so obsessed!!</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0scwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1g0smeb</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What I got done for Halloween </t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0smeb</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1g0v18v</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What shape? </t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5q7txh9890ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1g0umh3</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Halloween ready! Shoutout to Esthetics by Katie in Nova Scotia 👻🐈‍⬛🕷️</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ds4dolnr50ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1g0u9xl</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Too early?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0u9xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1g0u6r6</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Celestial Nails! 💅 </t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0u6r6</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1g0u0uc</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>3D Starry Night Nails</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/chm7bjau00ud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1g0tzer</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Chromatic Swirl Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ciz1b7f00ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1g0tr0p</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a jazzed up jelly nude </t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0tr0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1g0tkw7</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my first Russian manicure ahead of my wedding </t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dfqqdxbxztd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1g0tiyc</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Cute spooky nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tm6jwdzwwztd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1g0ta0t</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hermosas </t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfq8fl9yuztd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1g0t9t3</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Spooky vibes time!!</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0t9t3</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1g0s695</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Birthday Nails!!!</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0s695</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1g0s5yy</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Nail foil transfer sheet recommendations - not flowers/abstract</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g0s5yy/nail_foil_transfer_sheet_recommendations_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1g0s2jr</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Spooky season but make it Pink! Pretty proud of how I made them 3D! 👻</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cldvq29klztd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1g0s0ko</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Boo, you guys. </t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0s0ko</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1g0ptxa</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Ordered some custom press ons that are sticky?</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g0ptxa/ordered_some_custom_press_ons_that_are_sticky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1g0rcoj</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>my first nails art!! tell me some advice</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ggo1nkyfztd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1g0r81z</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>It’s been 3 weeks, Gel X</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0lqhxeyeztd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1g0r5ma</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying out this shape. </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0r5ma</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1g0r1kd</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yes or mess? </t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0r1kd</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1g0qs8d</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Back at it again</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0qs8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1g0qqce</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Last year’s Halloween nails were so cute</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2n6v3bw0bztd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1g0qfwg</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Do yall like my birthday nails!!</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0qfwg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1g0qafo</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Nail techs, what’s your biggest client peeve and how can we be better clients?</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g0qafo/nail_techs_whats_your_biggest_client_peeve_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1g0pqfz</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Nude spooks</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/im54um3g3ztd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1g0pk8a</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>My nails lady is a gift from the gods</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zamwu432ztd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1g0p9aw</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>I tried to make my nails look narrow - I was experimenting with pinching and "stilleto" dual forms.  Love the nude colour</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0p9aw</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1g0os3c</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Obsessed with my fall nails</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0os3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1g0o7vn</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Press ons I made for my bestie! ♥️</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0o7vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1g0nin1</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mine and my kiddos nails for concert </t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3lsimo8mytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1g0ncmi</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Little leopard vibes 🐆</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v769x2owkytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1g0nb7g</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Olive nails 🫒 </t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6c0uz8imkytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1g0mqnx</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🩸👻 Halloween Set 👻 🩸 </t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0mqnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1g0n4ar</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing a full set </t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0n4ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1g0n26y</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Very happy with this set 😊</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjwfjxvniytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1g0mlb6</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Now vs Then: Maleficent</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0mlb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1g0m7ez</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>I'm having an issue with attaching press on nails, I need advice</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g0m7ez/im_having_an_issue_with_attaching_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1g0m5c7</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Angora Cardi</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0m5c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1g0j9jl</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween (press ons from Temu) </t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0j9jl</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1g0l7xs</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Perfect for brautumn  🫒 </t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozo767jg4ytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1g0lyzi</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>So cute</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uc8lo5obaytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1g0k500</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I find going to the nail salon so confusing. </t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjmndcduvxtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1g0lqs3</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Halloween vibes🕷</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a75t8arl8ytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1g0h1pe</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Spooky season!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q97ijfwc4xtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1g0jefn</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>What shape should I get?</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0jefn</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1g0koma</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Cracked nail, any tips?</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0oerwha0ytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1g0lipe</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maybe some fun inspiration for someone out there. My wife's spooky scaries she got done. I like to send her ideas for her nails for inspiration and we go back and forth until she picks what she wants. I love  her new ones </t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4w7rjvzt6ytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1g0li5m</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Some of my Halloween nail art this year!</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0li5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1g0lecm</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Ready for spooky season 👻</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dhhzg4v5ytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1g0l6mk</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pixel pokeball over glitter &amp; chrome. i used my tiniest brush for this! </t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/br800l264ytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1g0ksiw</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Halloween Bat Claws by my super talented tech</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a376rhc51ytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1g0jxs8</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>I need a new design, can you give me ideas on what to do ✨🫶🏻✨</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abb1le98uxtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1g0jq3n</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Question About Nail Cutting</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g0jq3n/question_about_nail_cutting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1g0j6r6</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>advice?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0j6r6</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1g0ita5</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>What kind of nails is best for me?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g0ita5/what_kind_of_nails_is_best_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1g0i8gz</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Black, gold and brown combination. My favorite.</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h2ems1ufxtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1g0i22e</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall Nails </t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9whwq37extd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1g0hryw</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>It’s spooky time 🖤🩸</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0hryw</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1g0hcpk</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0hcpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1g0h1u5</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>What is gel overlay?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g0h1u5/what_is_gel_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1g0ggzd</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>New set I did 😇🩷</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qb34wg10ywtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1g0gf6k</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>october nails</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53qevzbgxwtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1g0gbhy</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How I discovered glitters :D </t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0gbhy</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1g0fa7i</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cherry bomb! 🍒 </t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vajgykfsjwtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1g0f921</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Me with the failed left hand press ons disaster here! I took your advice and tried just doing plain polish on my own nails. Please give me any advice and tips please! 🙏</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0f921</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1g0f67w</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Just trying something a bti different than what I usually get</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e12iaip9iwtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1g0eyo5</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Learning to do my nails</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0eyo5</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1g12oui</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nude velvet nails </t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c5d9um0oc2ud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1g12oul</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t xml:space="preserve">dreamy shifting magnetic </t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/or734ethc2ud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1g12hie</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Any opinions on Bio seaweed gel?</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g12hie/any_opinions_on_bio_seaweed_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1g129z4</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Dupe for Zenon lights lacquer</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g129z4</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1g11fgj</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The many faces of a single, spectacular multichrome 🌈 (paid/pr) </t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g11fgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1g10q9a</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>A serious haul from ILNP</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g10q9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1g10ckd</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>First time trying scoop marbling!</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1s18mkqm1ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1g0zivy</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>I'm in Love with my Halloween nails!</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0zivy</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1g0yv31</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sometimes Tomas and I have matching paws. </t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vyp8wid81ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1g0yu6o</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Mustard the Courage</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2pu6tn481ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1g0yn31</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Adding thermal pigment and searching for my dream thermal</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0yn31</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1g0ylln</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>LA Colors Vampy 🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0ylln</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1g0ylfr</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Staining concerns? Ilnp Ink</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydo9kyqq51ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1g0xxjp</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Adding thermal pigment and searching for my dream thermal</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0xxjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1g0xvpj</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Marble nails using silicone nail stamper</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0xvpj</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1g0xc4h</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>What’s your favorite polish of all time?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g0xc4h/whats_your_favorite_polish_of_all_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1g0wqkl</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What skin tone do yall think I have? Trying to find what polish colors look best on me! </t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0wqkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1g0w1nk</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>managed to grow out my natural nails for the first time in a long time, celebrating with a sheer sparkle</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0w1nk</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1g0v2rm</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>update on my smashed DVN bottle 🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86yh70hl90ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1g0v22x</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Multi-chrome magnetic in a deep oxblood jelly base? Ok fine I’ll break my no buy </t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0v22x</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1g0u7an</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>10 year old polish perfect for autumn!</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0u7an</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1g0u05b</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Favorite drug store brands?</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0u05b</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1g0tqen</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHHHH! </t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0tqen</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1g0tki2</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cold weather is upon us!!! Make sure to keep your hands moisturized </t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g0tki2/cold_weather_is_upon_us_make_sure_to_keep_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1g0talk</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>That shift 😍</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0talk</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1g0sydd</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>First holo taco order and I didn't even get holo</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l51vp41gsztd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1g0stwd</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>I love them!!!</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34s8voperztd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1g0sl7k</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Going for my Mysterious Uranus instead of her own today…</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gr2xamxkpztd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1g0skfq</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Can you make semi-hybrid with normal base, uv nail polish, and uv top coat?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g0skfq/can_you_make_semihybrid_with_normal_base_uv_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1g0sim3</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to find all the beautiful polish I the here in europe </t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g0sim3/how_to_find_all_the_beautiful_polish_i_the_here/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1g0s8bf</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Thoughts on this brick red almost brown shade?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0s8bf</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1g0rrby</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Dupe for Jewel Beetle</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xktt9t5jztd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1g0r45j</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>First fall mani of the year 💅🏻</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0r45j</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1g0qt5z</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>a little obsessed ngl</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0qt5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1g0qmqm</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Velvetized magnetics are now my obsession, THANKS A LOT REDDIT </t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/01qffcc8aztd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1g0qay2</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>HP Inspired</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0qay2</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1g0q72s</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Wanted candy apple, ended up with pickles</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rnc0xhnw6ztd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1g0pwy5</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Week 3 of nail polish jail</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4ztdww94ztd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1g0pjt4</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Ephemeral 💖</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0pjt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1g0p3r9</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glam Polish - I love you thorns and all </t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cvsi6v7fyytd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1g0nwnw</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Vampy Mooncat Mani</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvxtpfy9pytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1g0mpzc</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Lumen - Alpha from the big bad mystery set</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0mpzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1g0meit</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>8 out 10 spookies</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08b6nfwkdytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1g0maec</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Black, Red and naughty White</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om07ukvpcytd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1g0lwjz</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think Bunny approves my nail color? </t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0lwjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1g0k43t</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Spooky neons 👻💀</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0k43t</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1g0jjsc</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>ILNP Pool Party, Holo Taco Black Flake Taco, Sally Hansen Matte Top Coat 👻</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebyju433rxtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1g0jd9x</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>I'm Through Running Away</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0jd9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1g0jc0v</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>what's happening?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y82x8atbpxtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1g0i1vl</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Ghost Ship</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/483ksjd5extd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1g0hxx0</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Existence is terrifying </t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ia684s4dxtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1g0htow</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Kinda like this 🙃 🩵💜🩷</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7l9qp9zbxtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1g0hdk3</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>OPI x Wicked LE - Elphaba</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxs605zl7xtd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1g0faw6</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g0faw6/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1g0e9bf</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Definitely my fave Halloween Mani to date!</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0e9bf</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1g14azw</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>First nail set in uni</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g14azw</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1g0r1x0</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried nail art at home </t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/TBLicNaYK1o?si=H7aeB6azzVmtdWqO</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1g122tv</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Some halloweeen nails I’ve painted recently 🎨💅</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g122tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1g118xy</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Someone asked for glitter ✨ </t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zi1u08o8w1ud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1g10jxl</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>First time trying scoop marbling!</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nihzz16xo1ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1g0x13f</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1quijgxq0ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1g0untl</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Too early?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0untl</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1g0tn5p</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>First post..</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0tn5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1g0sz6m</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Olive nails 🫒 </t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ao8bvgmsztd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1g0sblv</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>My new Halloween nails! I am so obsessed! My nail tech is @nails_emmywynn on instagram!</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0sblv</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1g0qj15</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Pokémon nails </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0qj15</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1g0qbxi</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Modelones gel polish colours</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g0qbxi/modelones_gel_polish_colours/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1g0otg8</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finale Spooky 👻 nails </t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0otg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1g0oefw</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>My cutest set 💕</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z29gtdc6tytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1g0nsf7</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Pink drips and Scream mask!</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/so2kmekcoytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1g0nn90</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Halloween nails!</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4n8j57k7nytd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1g0nm2v</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Calling all press on gurus, I need your help!</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0nm2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1g0l3ck</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Pink halloween🎃👻🩷</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0l3ck</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1g0kl5k</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>PuppyCat🩷✨</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m9zmwkxizxtd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1g0j0im</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rock n roll </t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g0j0im</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1g0i1nn</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall Nails </t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwwaiyg3extd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1g0hng7</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Witchy kitty</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2lpurdbaxtd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1g0hl1y</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t xml:space="preserve">inspired by yin yang </t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gazcvkan9xtd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Oct 12 08:09:23 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_13.xlsx
+++ b/data/collected_data/2024_10_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1003"/>
+  <dimension ref="A1:C1172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17485,6 +17485,2879 @@
         </is>
       </c>
     </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1g1vags</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of this combination? </t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1vags</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1g1v2kx</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>💅</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1v2kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1g1uhp6</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>💜</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i0k8czdzw9ud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1g1uhhv</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>New french combination</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6c3zlnmww9ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1g1u7jv</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Just broke this 😔</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3xv7ql2t9ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1g1tuo3</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Southern California - Looking for a good nail salon</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1tuo3/southern_california_looking_for_a_good_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1g1tb6j</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>snoopy fall nails</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p831u4gkh9ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1g1syhl</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Y2K Pink Nails I Made💖💅🏼</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1syhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1g1souf</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>First time doing ny own nails!!</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jiabd9y2a9ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1g1sq0s</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Help with gel tips please</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1sq0s/help_with_gel_tips_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1g1snlm</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>vampy spiderwebs 🕸️✨</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1snlm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1g1sk6r</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Halloweenie!</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1sk6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1g1sejt</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red &amp; Black = a perfect combo </t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujv0zjlr69ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1g1ryrk</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love me a French tip </t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1ryrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1g1rlcz</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Halloween🧡</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48jfxz1qx8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1g1rfbd</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Fake or natural - and why?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1rfbd/fake_or_natural_and_why/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1g1rci2</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Halloween nails 👻</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/leznrpj0v8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1g1r09d</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>First DIY Press Ons… What do you think?</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rl1zzibcr8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1g1qodi</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Does this screen Halloween?</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/he5xwh6vn8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1g1qnmx</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>GelX w Tips</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brjhy3onn8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1g1q9bj</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enamorada </t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1q9bj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1g1q7wj</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>I think these are my favorite this year 🎃</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1q2uhl4j8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1g1q6mc</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spoopy nails </t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfq7qb2ui8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1g1q2fv</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>My Nail tech is amazing!!!</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1q2fv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1g1q1yz</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>My niece did my nails, very talented for being so little</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1cd501jh8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1g1q1rm</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>About form</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1q1rm/about_form/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1g1ppb8</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>New nails (dip)</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5dh3jqxd8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1g1pp5a</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice </t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6zhqcyvd8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1g1pij4</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>A year since I started doing my nails</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1pij4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1g1odok</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>nail filing</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1odok/nail_filing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1g1pgf0</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Spider web nails</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3mnzqhdb8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1g1p2vj</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails by kristinaghita on instagram. INSANE </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1p2vj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1g1pevm</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Did these today!</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1pevm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1g1pch4</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Elegant nail art </t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3uuw2s8a8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1g1p3wy</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Oh noooo I get it now </t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czquwtpu78ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1g1ozny</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How are you doing your nails without a gel lamp? </t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngvsidrn68ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1g1oibo</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Another twist on a classic for Halloween</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnlbvsdw18ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1g1ofhp</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>First spooky set of the season💕👁️🖤</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npdo2om518ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1g1ob7j</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>My nails cracked 😭 what can I do?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckf6k5qzz7ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1g1o2s6</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>guys.. look at these, I love them so much 🩸♥️💉</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kyd9rxvpx7ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1g1o2e7</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>how to protect a hangnail when removing polish?</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1o2e7/how_to_protect_a_hangnail_when_removing_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1g1nc8j</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Best metal press ons for my girlfriend?</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1nc8j/best_metal_press_ons_for_my_girlfriend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1g1ng02</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>3d halloween nails done by me!</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1ng02</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1g1n90k</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Thoughts and advice?</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1n90k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1g1n0pb</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Is this lifting?</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1n0pb/is_this_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1g1mkay</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>friend whos learning did this set :3</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1mkay</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1g1m51r</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need so much more practice 🫣 But I love them anyways. First fall set! </t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wggnyp3bg7ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1g1lwbu</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Love how they turned out!</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kgcari9e7ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1g1ls5q</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>My Halloween nails 🕸️🕷️</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8x5g7nbd7ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1g1lbrb</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Halloween nails done by me on me 😅</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzgg2vyg97ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1g1k2e7</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>how do these look?</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1k2e7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1g1j9p1</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thermal ghosties </t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1j9p1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1g1jepw</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Drippy Set</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1jepw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1g1l167</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>It was fun to make them 🫠💅🏻</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r930w5u177ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1g1jvk5</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Teach me your ways</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gswor19jx6ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1g1kl6b</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>I bought cheap stick on nails. I loved the matt blue. But they started breaking… so I had to cut the team. 😅</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1kl6b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1g1kg8m</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel cleaner alternative? </t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1kg8m/gel_cleaner_alternative/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1g1kfax</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>10 days growth - how to keep up with nails??</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1kfax</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1g1kbeq</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Thoughts for this newbie?</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1kbeq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1g1k8ij</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Does anyone have a recommendation?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvdhz3dg07ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1g1jz3k</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>birthday nails</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1jz3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1g1jgcb</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>tips on how to make this french gradient on my natural nails?</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39iw6nf2u6ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1g1jdpt</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Color changing/glowing ghosties for October 👻</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1jdpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1g1j67n</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>If budget wasn’t a problem what would be your dream Halloween set? (Current set I’m working on)</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1j67n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1g1iznw</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>I tried a deep red on my nails IDK HOW I FEEL YALL 😭😭</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1iznw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1g1irb6</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Cured BIAB dipping</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1irb6/cured_biab_dipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1g1ik17</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat Eye Polish </t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2vqw0owm6ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1g1iiuy</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Spooky season nails: check 🤣</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1iiuy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1g1hl3v</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Thoughts on dip?</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1hl3v/thoughts_on_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1g1hktc</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>I'm simple, I like chocolate ☕🍁🍂</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1hktc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1g1h50m</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>용</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1h50m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1g1h409</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>🩸 ILNP Bitten 🦇 So juicy and plump and vampy 💀👻🪦❤️</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1h409</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1g1h0t5</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Do you tip your nail tech..?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1h0t5/do_you_tip_your_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1g1fxng</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>getting my nails done professionally for the first time, i have a question</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1fxng/getting_my_nails_done_professionally_for_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1g1ggju</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Short Red Cat Eye</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0naa9b366ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1g1ge9i</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1fng4el56ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1g1gd8l</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>One year difference as a beginner nail tech!!</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1gd8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1g1g7lu</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>First time I've done semi-permanent ones</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/js4mffx546ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1g1g7et</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye vampire nails (: i did on myself. </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1g7et</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1g1fvcw</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Sharing my spooky manicure</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1fvcw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1g1f48n</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long chubby fingers </t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43usgd2mv5ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1g1ey3n</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>By far the cleanest manicure I’ve ever done on myself</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1ey3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1g1dumj</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First self-painted set! 💅 </t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1dumj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1g1dpr5</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Palette cleanser 🤍</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c47b2mtok5ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1g1d9pj</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Halloween nails! </t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1d9pj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1g1cus4</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Thermal gel</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1cus4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1g151q5</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m learning to do my nails </t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g151q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1g16xyu</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Went for a classic autumnal vibe 🍂✨</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g16xyu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1g1c72u</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Polish recommendation for a protective coat for healthy nails?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1c72u/polish_recommendation_for_a_protective_coat_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1g1cnax</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail biting journey from current to where I started! </t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1cnax</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1g1cgu7</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Cute lil spooky ghosties</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l20wnpp5b5ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1g1cgq8</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Victorian vampy vibes set ? I don't have any ideas for a name set 😅</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1cgq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1g1cesd</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>did a twist on a classic set &amp; i kinda love it</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1cesd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1g1cek0</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Tea patch- how did I do?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1cek0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1g1besz</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tortoise she’ll vibe, but black and gold </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1besz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1g1az1q</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Nail help!</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1az1q/nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1g1avl8</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Woollybear Nails!</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1avl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1g1aqu7</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>First time getting acrylics for spooky season</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1aqu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1g1amnz</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I was being a little difficult but my tech absolutely nailed this set. </t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1amnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1g19ojh</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>I’m a nail art newbie, but I’m very happy with how these turned out! 💖</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8s8qxiro4ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1g1txwv</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Orly Red shades Swatch Please?🥺</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g1txwv/orly_red_shades_swatch_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1g1th3p</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Does LynB regularly edit swatches??</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmmioq0nj9ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1g1s5i4</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Is it giving Halloween?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1s5i4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1g1rbwe</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it bad to keep OPI nail envy on for more than a week long? </t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3cdurnsu8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1g1q768</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>ILNP Venom 🐍✨</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1q768</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1g1px9p</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>ILNP High Dive vs. Holo Taco Peri-Social</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1px9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1g1psnu</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does Lyn B Designs offer online order cancelations or edits? </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g1psnu/does_lyn_b_designs_offer_online_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1g1pc1q</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for JL Lacquer Newport</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g1pc1q/looking_for_a_dupe_for_jl_lacquer_newport/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1g1p2wf</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Goddamnit 😭 I love it</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cpjiv4k78ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1g1oc49</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Holo Taco @ Ulta</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uiohpbc808ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1g1ntr6</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>First Time Stamping!</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avo1u6efv7ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1g1nnwj</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Much Lava to You (aka dark and spooky rainbows 🌈)</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/btgjnuvwt7ud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1g1mtjz</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Holo and layered flakies for sparkly galaxy nails 🌌💅🏻</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8qvucho1m7ud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1g1ment</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Sagebrush 🍃</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1ment</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1g1mcz1</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simplicity </t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8w4n4x7i7ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1g1m389</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>I love this gorgeous red from Cracked!</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1m389</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1g1ly7x</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Good quality swatch sticks UK?</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g1ly7x/good_quality_swatch_sticks_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1g1lx1t</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>A perfect fall combo 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1lx1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1g1lvgv</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Which cuticle remover is the most gentle?</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g1lvgv/which_cuticle_remover_is_the_most_gentle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1g1kn85</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Do I have a favourite colour/combo rn? 😂😅</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1kn85</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1g1kmuq</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>do you guys know of any dupes for this polish that's coming out tomorrow?</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ehft6dq37ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1g1k7kj</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>My husband: “I got you this nail polish because it made me think of Halloween” 🥰 🎃🧡</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pvro7t807ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1g1jwu4</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Breaking News</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1jwu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1g1ibey</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You have a $40 budget for Sally’s </t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g1ibey/you_have_a_40_budget_for_sallys/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1g1hvsa</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>How do you guys store your fake nails? What containers / organizers do you use?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g1hvsa/how_do_you_guys_store_your_fake_nails_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1g1hq9u</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>CND Stickey Base Coat discontinued?</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g1hq9u/cnd_stickey_base_coat_discontinued/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1g1h37y</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>🩸 ILNP Bitten 🦇 So juicy and plump and vampy! 👻💀🪦❤️</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1h37y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1g1gu6p</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Are there any magnetic techniques that are easier than others?</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dknd10y396ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1g1gsz6</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>I cannot resist a good frosted metal 🪩</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxl6292u86ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1g1fz0f</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Orchid Escape </t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pa3hejff26ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1g1fmle</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Hopping on the orange/purple train 🧡💜🚂</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1fmle</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1g1ei5t</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Anyone else jump on the LynB sale?</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqanvm8uq5ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1g1dqmn</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>The Diabolical Mojo Jojo!!</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/GzdYClh.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1g1d3fz</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>I Appreciate an Appropriately Named Nail Polish - Autumn by Zoya</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4asrdh1g5ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1g1cuzg</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Lurid does it again!</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1cuzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1g1cqxz</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Swatching journal</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g1cqxz/swatching_journal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1g1cev8</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>LynB Designs</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t93l92oqa5ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1g1ca1r</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>I Scream Party 👻🍦</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1ca1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1g1c5er</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>🌈National Coming Out Day🌈</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1c5er</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1g1c267</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is my OPI christmas gone plaid a knockoff? font is different than the others and the underside label looks different </t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1c267</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1g1bpyy</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>grave consequences by polished for days 🕸️</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7h3re7af55ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1g1boys</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>ILNP Hidden Treasure</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1boys</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1g1ba1a</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Beetlejuice Beetlejuice Beetlejuice 💜💚</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1ba1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1g1b5n3</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I clearly have a type </t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1bxuwlex05ud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1g1anv2</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Mooncat love</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73ozrabww4ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1g1aez7</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Crème polish recommendations</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fc60qhe0v4ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1g1abuq</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Junji-ito nails</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1abuq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1g1ab91</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>ILNP Hex (#2)</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1ab91</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1g19tip</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bday mani </t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/atsic0hzp4ud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1g18a89</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of my favorite autumn polishes </t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66x4fag1c4ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1g17yix</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>What are the best bees knees polishes?</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmuvo1nt84ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1g17fjq</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Love the polish but…</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g17fjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1g179il</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Halloween mani 🕸️🕷️🕸️</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g179il</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1g1rx13</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My spooky Disney themed set </t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6p4pdka19ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1g1qfrw</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural nails, non-gel polish </t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3x811q7l8ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1g1pjnf</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>A year since I started doing my nails</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1pjnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1g1pfwt</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What she asked for vs what she got! </t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1pfwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1g1o3y4</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloweenie! </t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1o3y4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1g1ku2r</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky nails! </t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lchmpcme57ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1g1jfy4</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>How do I get these lines and curves to be more uniform?</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1jfy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1g1jajs</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>I painted Halloween Moo Deng: “Boo Deng!”</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h59a046ss6ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1g1j4ou</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thermal Ghostly Nails </t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1j4ou</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1g1hp6r</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>My not so spooky October nails 👻🎃</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1hp6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1g1h6it</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>용</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1h6it</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1g1dscw</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Celestial Nails! 💅 (done by myself at home)</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1dscw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1g1c9zi</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Victorian vampy vibes set ? I don't have any ideas for a name set 😅</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1c9zi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1g1brle</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Shining Nails</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1brle</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1g1bftv</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>My grandmother wanted to wear her nails for Halloween and I did them for her.</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwc7lcb635ud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1g16pju</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Went for a classic autumnal vibe</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g16pju</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Oct 13 08:09:44 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_13.xlsx
+++ b/data/collected_data/2024_10_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1172"/>
+  <dimension ref="A1:C1370"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20358,6 +20358,3373 @@
         </is>
       </c>
     </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1g2jmtj</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done today 💅 </t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbxx8h86ygud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1g2jkfx</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>First try!</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t41phwq8xgud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1g2jjym</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Third set on myself. Am I getting somewhere? 😂 </t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oyy6fs82xgud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1g2iqu7</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Did some simple nails for a friend</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2iqu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1g2imi0</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>How to fix this?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2imi0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1g2iemh</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Category is: autumnal floral</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4oilt4zaigud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1g2iawx</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>some of my recent sets ✨</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2iawx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1g2ibw1</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>No longer have FOMO seeing all the cute Halloween nail designs 👻😂</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oieg5z3ehgud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1g2him2</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>flash on vs off for nail pics? ✨️</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2him2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1g2hdbs</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>My first Halloween design Press on nail set 🎃👻 What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2hdbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1g2h8oi</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Press on Nails by me 🥺</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2h8oi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1g2ghan</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Which one was better?</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2ghan</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1g2g03a</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My current nails (by me) </t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kplv56fhrfud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1g2gabm</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Autumn colored Halloween nails 🤎🕸️👻</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2gabm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1g2eajo</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky season </t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nylgbilq9fud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1g2fyex</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>PomPomPurin mushroom press ons</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5czzh4o0rfud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1g2dumk</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My son is graduating from Navy boot camp next week! </t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5dg30485fud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1g2dddi</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>I did my own nails for the first time since high school. Would love some constructive criticism!</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2dddi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1g2fkg0</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Mom &amp; I got our nails done 🧡💕</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ldctekymfud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1g2fkce</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Red chrome</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yyienybxmfud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1g2eydc</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Nail techs UK using fresha</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g2eydc/nail_techs_uk_using_fresha/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1g2ev55</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Did my nails! Stars and bows 🎀</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2ev55</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1g2esf3</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>My Halloween dreams come true!!!</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2esf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1g2ena9</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Loving the color changing polish</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0ciwhiedfud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1g2elbe</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Blue cat eye😍</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/edf1uhfucfud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1g2eemr</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set 💅🏻 </t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2eemr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1g2eanv</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>What to do</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2eanv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1g2dw4i</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Is this how almond nails are supposed to look/feel?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2dw4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1g2dsob</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>First time doing my nails myself</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2dsob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1g2ds49</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Demure Halloween?</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2ds49</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1g2dp7l</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>missing this set 🖤</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2dp7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1g2do7x</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>New nails classic set</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxymoyzg3fud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1g2de82</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>My WIP Halloween nails are going well.</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2de82</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1g2dcsu</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Naked natural nails.</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2dcsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1g2d7e5</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Magnetic jelly nails on a friend using Gel X (done by me✨️)</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2d7e5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1g2c8rr</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>It's Halloween it's Halloween 🎃🎃</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/es3xb30rpeud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1g2bxt8</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Halloween press ons from Olive &amp; June</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8x7ho6ymeud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1g2buyc</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>did my nails today 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2buyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1g2bkz8</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>I just did my nails for the first time</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2bkz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1g2bi38</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Got my spooky set today 👻🖤</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wn7cgoavieud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1g2b1bx</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>ILNP - Zero Degrees❄️</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2b1bx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1g2azpk</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Halloween nails done by me! 🥹</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l16jhtg5eeud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1g2ardj</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>matching with the ocean today💙</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2ardj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1g2anny</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">October nails </t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6yfwtp78beud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1g2ak1h</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween set is done </t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j16ftyycaeud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1g2acca</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>New Set Every Week?</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g2acca/new_set_every_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1g2a91w</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set for my birthday Monday </t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/druwto4o7eud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1g2a0if</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Navy blues </t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2a0if</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1g29z30</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>so proud of myself</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g29z30</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1g29rtn</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Had an accident and split my nail down to almost the quick, just a few questions.</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g29rtn/had_an_accident_and_split_my_nail_down_to_almost/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1g29rae</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>💚Nails💚</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u28oas9f3eud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1g29quc</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New York Red </t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3xbfayb3eud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1g29g24</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Black kitties for Halloween 😻</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g29g24</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1g29fc2</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>I love marbled!</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g29fc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1g29bj4</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>My new color of nails</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0f2v0jqzdud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1g29atg</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Fake Nails Question...</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g29atg/fake_nails_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1g29215</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Gel polish on natural nails - regret the color</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgjwc22gxdud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1g28v6a</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fav fall color! 🍒☕️ </t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkflbrpsvdud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1g28rsa</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just wanted to share </t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g28rsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1g28r5m</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Nails I’m Making For Someone  🖤🩸🖤🩸🖤🩸🖤</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvkr94ztudud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1g28n8h</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>🍒☕️</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8sd9x8wtdud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1g28eug</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Jessica Rabbit nails🎃</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymfg3fnyrdud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1g287h9</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>My bloody nails</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7dyve108qdud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1g27kaa</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>New set 💗</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g27kaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1g27ivh</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Simple &amp; clean in green 💚</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g27ivh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1g27gl6</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thought I wanted square </t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g27gl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1g275ox</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>How long does the teabag method last?</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g275ox/how_long_does_the_teabag_method_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1g26wso</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Halloween nails 👻</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ec65f6nifdud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1g25uhz</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glow in the dark nails </t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g25uhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1g25sqk</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>God bless my tech</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsz0s8af6dud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1g25r7l</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>hi guys! new to manicures, looking for monthly price</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g25r7l/hi_guys_new_to_manicures_looking_for_monthly_price/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1g25nkb</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Halloween + Vegas</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozsn7gy95dud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1g25def</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>2nd character nail set ki</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqbqu18z2dud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1g259vj</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Newbie</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g259vj/newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1g24qo4</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>First time doing 3D nail art how did I do ??🐙🐙</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g24qo4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1g24fgg</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail design for this week </t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ys4wu37vcud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1g248ji</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>I’m in love, I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g248ji</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1g23xqa</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>red or black?</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imyqd0a4rcud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1g1y4k8</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>I asked my nail tech to paint my cat and she delivered!</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1y4k8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1g239rl</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>did my own nails for the first time… please roast me 🤣</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g239rl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1g235ke</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Someone pls give my there honest opinion on these colors together </t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyej4lgnkcud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1g234ke</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spider Mickey Mouse </t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yp2usg1hkcud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1g22xmu</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>I love seeing natural long nails without polish</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5gzqgakicud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1g22ttq</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Day 1 of natural nails with charms</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g22ttq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1g22ne3</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>are there any teenager-friendly job ideas where you can still have nails?</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g22ne3/are_there_any_teenagerfriendly_job_ideas_where/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1g22e38</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Happy Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g22e38</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1g1w9um</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Thoughts on Butter London Signature Glass File?</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1w9um/thoughts_on_butter_london_signature_glass_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1g1wu51</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Saw them on pinterest and had to get them done</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1wu51</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1g1z3bv</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>acrylic nail damage</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g1z3bv/acrylic_nail_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1g226l8</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Chains and roses</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lisoqgnccud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1g21y2x</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>I liked and I didn't like... you know when you're getting used to the color...</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3z6j0ahpacud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1g21n9b</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky nails </t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g21n9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1g21bty</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Got them done for 50€- worth it? They’re acrylic 🔪🩷</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6kz7v2i5cud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1g21a1n</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need recommendations for affordable long lasting everything! (Base, top, polish, nippers, cuticle oil) </t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g21a1n/need_recommendations_for_affordable_long_lasting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1g20vcq</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my nails halloween themed </t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g20vcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1g20nya</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are my nails pretty😇
+</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0onm8mwnzbud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1g1zfn2</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Got my nails done (by me)</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6w0157g3obud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1g1zawk</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>I love lizards 🥰</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1zawk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1g1z7uy</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Nudes will always hit 🌸</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pm7nerdrlbud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1g1z3uc</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Guess how much these cost</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/epeaozhokbud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1g2jdbl</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Gel dupe for Nails Inc Knightrider’s Street?</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2jdbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1g2icof</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Give me your favorite unique indie brands to browse ☺️💅</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g2icof/give_me_your_favorite_unique_indie_brands_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1g2hzpg</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pick my next color for me </t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gop4981hdgud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1g2hl3p</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Why do my nails look so messy?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szbawd0q8gud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1g2gi9l</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>ILNP Sabrina (matte)</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/igghwfn4wfud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1g2fxgr</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Estoy Polishes</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g2fxgr/estoy_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1g2ft8p</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Broke my nail playing volleyball 🗿</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2ft8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1g2f1xv</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Magnetic comparisons/Dupes</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2f1xv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1g2exho</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>I'm in pain</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvpxmo79gfud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1g2exfo</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Love this blue</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3g1aevp8gfud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1g2ejql</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>over the moon 🐰🌕</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wliqp7ecfud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1g2edcp</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>These are all the same polish 😍</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2edcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1g2e37t</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Whatcha Nightshade </t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9rem6c4n7fud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1g2dqun</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Amazing color for fall!</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2dqun</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1g2dpfo</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Clionadh Hot Toddy</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qs6otk9t3fud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1g2dnej</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat 🌙 </t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gy15vf793fud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1g2dlq2</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer- I'm a Haunt Mess</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/doaboz0t2fud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1g2d3w5</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Deep dive: the worlds brightest glow in the dark polishes</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2d3w5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1g2cn9a</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Riding Sleeping Bags Down the Stairs</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2cn9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1g2bxcn</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Fall 🍂🍁🍃</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2bxcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1g2bp22</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>dark matter 🪐</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wk1t1dkokeud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1g2bdzm</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>You shall not pass to walk on the wild side</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/017k87elheud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1g2b64k</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Cirque Colors new magnetics are absolutely stunning! Fool's Paradise, Pipe Dream, and Wishful Thinking (+ Paradox)</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2j3eket7deud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1g2b3cb</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>ILNP - Zero Degrees❄️</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2b3cb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1g2awl8</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matched my mani to my saree. Camera doesn’t agree 🙃 </t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lqczef9deud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1g2a7kl</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Help! I can’t pick a blurple!</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g2a7kl/help_i_cant_pick_a_blurple/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1g29y63</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Obsessed 🪐</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g29y63</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1g296ok</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Arcana Lacquer-Lash of Bhaal vs Fancy Gloss-Midnight Veil</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g296ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1g287y1</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Fun nails for the long weekend</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9g6z84xbqdud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1g284wr</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else have nostalgia shades? Picked up a new bottle of one of my first polishes </t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xecs8dnpdud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1g282x3</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Essie Yes I Canyon</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhjeatj6pdud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1g27zcp</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>She’s so beautiful 🥹😭</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g27zcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1g27wur</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>simple fall skittle</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zeqz4vprndud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1g27ra8</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>If you had to restart your nail polish collection, how would you go about it?</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g27ra8/if_you_had_to_restart_your_nail_polish_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1g27i9c</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need to be more mindful about the polish I buy. </t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g27i9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1g27ds5</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Anyone know of a polish in this shade with the green/pink shift?</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kz0alogajdud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1g26wdu</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Spotted Psilocybin 🍄</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g26wdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1g26si9</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help match my car please! </t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lr3rgyziedud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1g26pkp</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Glitter on the highway 🎶</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g26pkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1g26o32</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>What’s an iridescent mermaid nail polish that looks like this?</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g26o32</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1g26g57</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Help - topper</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g26g57</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1g25mg8</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Anyone know where I can find this glossy emerald green color but NOT in a gel polish?</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x82z9ow05dud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1g25l3h</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>🇨🇦 Thanksgiving Mani</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g25l3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1g25j71</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>ILNP’s Poison might be the prettiest red polish I own 🍎❤️</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g25j71</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1g25fab</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>ILNP - Cameo</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g25fab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1g23y5p</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Rose kaolin (cirque colors) dupe?</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g23y5p/rose_kaolin_cirque_colors_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1g22xh5</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Heck yeah!</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1junqj0vicud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1g22s6s</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KB shimmer sugar spice and everything nice </t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bd6flq8nhcud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1g22msn</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Creative store display</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnnazuxdgcud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1g22fsn</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>out-pruglied myself</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g22fsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1g22bva</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>The only thing cheering me up today is my polish</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g22bva</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1g223sl</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you ever feel guilty for buying a polish and never wearing it? </t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ev7yuoyzbcud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1g21ooz</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Are some magnetic polishes just worse than others?</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g21ooz/are_some_magnetic_polishes_just_worse_than_others/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1g21k81</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Maelstrom 🧜🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g21k81</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1g21jy5</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Skittle ILNP Harvest Collection + Holo (because duh)</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g21jy5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1g217ci</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need good recommendations on long lasting everything! Base, top, color, cuticle oil, nippers </t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g217ci/need_good_recommendations_on_long_lasting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1g20gov</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>This nailpolish is SO pretty!!</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g20gov</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1g20gbe</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>ILNP polishes to satisfy Holo Taco Birthday Gemstones craving</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g20gbe/ilnp_polishes_to_satisfy_holo_taco_birthday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1g20crw</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Lots of Zoya at Tjmaxx?</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g20crw/lots_of_zoya_at_tjmaxx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1g20430</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally figured out how to do the tortoise look! Very 2014, but I love how these turned out. </t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gzcf3vaubud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1g200h7</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Cirque Lucky Jelly is the perfect red 😍</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g200h7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1g1zy0d</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Jade manicure</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0nf6ndysbud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1g1zx2z</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Skittle for autumn!</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3qjauepsbud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1g1za5b</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Whatcha Velvet Magnet Tool</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1za5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1g1whm0</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>What does BNNB mean?</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g1whm0/what_does_bnnb_mean/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1g1wghs</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>H&amp;M beauty nail polish ‘December Dawn’</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1wghs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1g1wb5o</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Butter London Signature Glass File</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g1wb5o/butter_london_signature_glass_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1g1vx31</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>🌈☀️🌡️The Science of Nail Polish: Thermals and Solars 🌡️☀️🌈</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g1vx31/the_science_of_nail_polish_thermals_and_solars/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1g2gy1c</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>After getting them done 💜💚</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icnonanl1gud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1g2gx5z</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Before getting them done </t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wec0onbc1gud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1g2gwcc</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>I can’t pick what I want for my wedding nails</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2gwcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1g2gfey</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Nail night!</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcnj03azvfud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1g2g5s1</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Shining design </t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6i65ss4tfud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1g2fzba</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>After 💚💜</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dknm2ip9rfud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1g2fxpu</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Before 🥱</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bu911evsqfud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1g2fxgo</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>How do I use nail sculpting gel?</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g2fxgo/how_do_i_use_nail_sculpting_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1g2fowk</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tentacles 🦑 </t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2fowk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1g2ffsb</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Roku City</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2ffsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1g2fap9</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Laugh Now, Cry Later 🤡</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2fap9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1g2dptw</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>pleasing my clients who like to be in trend, I share a little of my work constructive criticism girls</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwgkngkx3fud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1g2ddjb</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I go into nail school? </t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2ddjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1g2cyvg</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So like… do I go to a hospital or what? 🤔 </t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2cyvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1g2caao</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Happy Halloween!</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2caao</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1g2bp7l</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Retention </t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2bp7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1g2bo9w</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>coraline vibes</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2bo9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1g2aecy</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>New press on nails for Halloween what do you think?</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bf1xqdbz8eud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1g29raa</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0h5xeaf3eud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1g283bf</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Spooky Toes!</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0tokzn9pdud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1g27v3u</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>miffy!!</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5c054mwdndud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1g26b2w</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Halloween nails❣️</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tifh6pwladud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1g24ogo</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I organize a Zombie Bar Crawl in my city and my girl @nailedtothecounter set me up right </t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2r17yg8xcud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1g2410c</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Photo dump of my nails ✨</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g2410c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1g23jqu</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>I did a tutorial on my witch nails!!</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g23jqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1g23hv3</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My longest nails yet and first time using magnetic polish </t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6bapymhncud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1g20ioo</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Spooky spider nails</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g20ioo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1g1yjae</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>HELP! I think I hate my wedding nails. Should I redo them? It’s tmrw 😅</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1yjae</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1g1xw30</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Did my nails Halloween themed this time</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1xw30</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1g1x7yj</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>My friends let me do their nails✨</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g1x7yj</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>